<commit_message>
update the number of weekly doses by age
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccination_12dose_05031031.xlsx
+++ b/data/vaccine/vaccination_12dose_05031031.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iyunjeong/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D44B2F-17AB-9A4E-AE42-64C3BA07B3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E28AF22-E23C-A041-92DA-62D6370B52D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19660" yWindow="2120" windowWidth="21300" windowHeight="13680" activeTab="1" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
   </bookViews>
@@ -183,12 +183,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -536,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2E4180-383F-D540-B7B7-6029C29EA127}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,6 +1380,70 @@
         <v>1885923</v>
       </c>
     </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>44494</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5">
+        <v>236431</v>
+      </c>
+      <c r="D27" s="5">
+        <v>6880268</v>
+      </c>
+      <c r="E27" s="5">
+        <v>5877730</v>
+      </c>
+      <c r="F27" s="5">
+        <v>7411175</v>
+      </c>
+      <c r="G27" s="5">
+        <v>8165973</v>
+      </c>
+      <c r="H27" s="5">
+        <v>6793813</v>
+      </c>
+      <c r="I27" s="5">
+        <v>3514175</v>
+      </c>
+      <c r="J27" s="5">
+        <v>1888549</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>44500</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0</v>
+      </c>
+      <c r="C28" s="5">
+        <v>430369</v>
+      </c>
+      <c r="D28" s="5">
+        <v>6941446</v>
+      </c>
+      <c r="E28" s="5">
+        <v>5921453</v>
+      </c>
+      <c r="F28" s="5">
+        <v>7442380</v>
+      </c>
+      <c r="G28" s="5">
+        <v>8186088</v>
+      </c>
+      <c r="H28" s="5">
+        <v>6804755</v>
+      </c>
+      <c r="I28" s="5">
+        <v>3518256</v>
+      </c>
+      <c r="J28" s="5">
+        <v>1891250</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1388,10 +1453,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA06488B-6AE1-6D45-B18E-AB20070D0C15}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1996,31 +2061,31 @@
       <c r="C22" s="2">
         <v>15805</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <f>2224897-3141</f>
         <v>2221756</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <f>2252640-910527</f>
         <v>1342113</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <f>2347504-300291</f>
         <v>2047213</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <f>3936454-112754</f>
         <v>3823700</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="2">
         <f>6235304-76029</f>
         <v>6159275</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="2">
         <f>3360396-10483</f>
         <v>3349913</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="2">
         <f>1796798-2159</f>
         <v>1794639</v>
       </c>
@@ -2035,31 +2100,31 @@
       <c r="C23" s="2">
         <v>15853</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <f>2410388-3215</f>
         <v>2407173</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <f>2375739-914613</f>
         <v>1461126</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <f>2551264-303949</f>
         <v>2247315</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <f>4467926-115524</f>
         <v>4352402</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="2">
         <f>6251902-76873</f>
         <v>6175029</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="2">
         <f>3365374-10601</f>
         <v>3354773</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="2">
         <f>1799471-2226</f>
         <v>1797245</v>
       </c>
@@ -2074,31 +2139,31 @@
       <c r="C24" s="2">
         <v>15926</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <f>2873413-3289</f>
         <v>2870124</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <f>2701945-922332</f>
         <v>1779613</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <f>3098638-310289</f>
         <v>2788349</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <f>6815806-120220</f>
         <v>6695586</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="2">
         <f>6319137-78130</f>
         <v>6241007</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="2">
         <f>3383937-10843</f>
         <v>3373094</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="2">
         <f>1807386-2450</f>
         <v>1804936</v>
       </c>
@@ -2113,31 +2178,31 @@
       <c r="C25" s="2">
         <v>16053</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <f>3730535-3370</f>
         <v>3727165</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <f>3272712-927185</f>
         <v>2345527</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <f>3940023-313977</f>
         <v>3626046</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <f>7763055-122683</f>
         <v>7640372</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="2">
         <f>6481623-78793</f>
         <v>6402830</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="2">
         <f>3420433-10950</f>
         <v>3409483</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="2">
         <f>1820266-2489</f>
         <v>1817777</v>
       </c>
@@ -2152,33 +2217,111 @@
       <c r="C26" s="2">
         <v>16163</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <f>4530087-3467</f>
         <v>4526620</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <f>3949447-930964</f>
         <v>3018483</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <f>5008953-316891</f>
         <v>4692062</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <f>7836973-124828</f>
         <v>7712145</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="2">
         <f>6574635-79430</f>
         <v>6495205</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="2">
         <f>3440746-11084</f>
         <v>3429662</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="2">
         <f>1828611-2575</f>
         <v>1826036</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>44494</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <v>16329</v>
+      </c>
+      <c r="D27" s="2">
+        <f>5407291-3543</f>
+        <v>5403748</v>
+      </c>
+      <c r="E27" s="2">
+        <f>4692700-934165</f>
+        <v>3758535</v>
+      </c>
+      <c r="F27" s="2">
+        <f>6053381-319385</f>
+        <v>5733996</v>
+      </c>
+      <c r="G27" s="2">
+        <f>7893163-126532</f>
+        <v>7766631</v>
+      </c>
+      <c r="H27" s="2">
+        <f>6637674-79918</f>
+        <v>6557756</v>
+      </c>
+      <c r="I27" s="2">
+        <f>3455989-11188</f>
+        <v>3444801</v>
+      </c>
+      <c r="J27" s="2">
+        <f>1836181-2650</f>
+        <v>1833531</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>44500</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>16553</v>
+      </c>
+      <c r="D28" s="2">
+        <f>6308914-3648</f>
+        <v>6305266</v>
+      </c>
+      <c r="E28" s="2">
+        <f>5410439-936993</f>
+        <v>4473446</v>
+      </c>
+      <c r="F28" s="2">
+        <f>6982173-321630</f>
+        <v>6660543</v>
+      </c>
+      <c r="G28" s="2">
+        <f>7952797-128071</f>
+        <v>7824726</v>
+      </c>
+      <c r="H28" s="2">
+        <f>6678560-80450</f>
+        <v>6598110</v>
+      </c>
+      <c r="I28" s="2">
+        <f>3467744-11283</f>
+        <v>3456461</v>
+      </c>
+      <c r="J28" s="2">
+        <f>1843298-2688</f>
+        <v>1840610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 1st, 2nd and add 3rd
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccination_12dose_05031031.xlsx
+++ b/data/vaccine/vaccination_12dose_05031031.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iyunjeong/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjlee/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E28AF22-E23C-A041-92DA-62D6370B52D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7A784E-8E6C-7241-9C8E-DC66A3E35265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19660" yWindow="2120" windowWidth="21300" windowHeight="13680" activeTab="1" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
+    <workbookView xWindow="8600" yWindow="620" windowWidth="28800" windowHeight="15740" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
   </bookViews>
   <sheets>
     <sheet name="1st dose" sheetId="1" r:id="rId1"/>
     <sheet name="2nd dose" sheetId="2" r:id="rId2"/>
+    <sheet name="3rd dose" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -92,8 +96,37 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={64D7B1B1-E6AF-F24D-9648-FE478B623C74}</author>
+    <author>tc={C7F97C34-3911-E94C-817A-1FDE668F5392}</author>
+  </authors>
+  <commentList>
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{64D7B1B1-E6AF-F24D-9648-FE478B623C74}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    12-17세: 12,596
+미포함</t>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="1" shapeId="0" xr:uid="{C7F97C34-3911-E94C-817A-1FDE668F5392}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    12-17세: 13,051
+미포함</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>date</t>
   </si>
@@ -132,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,13 +194,31 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -183,13 +234,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -206,6 +261,33 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="1st dose"/>
+      <sheetName val="2nd dose"/>
+      <sheetName val="3rd dose"/>
+      <sheetName val="2nd dose_prev"/>
+      <sheetName val="Sheet4"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="2">
+          <cell r="B2">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,12 +617,25 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D18" dT="2021-09-03T10:28:52.34" personId="{11A4F5F0-4273-964A-87D2-52A5A4679086}" id="{64D7B1B1-E6AF-F24D-9648-FE478B623C74}">
+    <text>12-17세: 12,596
+미포함</text>
+  </threadedComment>
+  <threadedComment ref="D19" dT="2021-09-03T10:31:16.26" personId="{11A4F5F0-4273-964A-87D2-52A5A4679086}" id="{C7F97C34-3911-E94C-817A-1FDE668F5392}">
+    <text>12-17세: 13,051
+미포함</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2E4180-383F-D540-B7B7-6029C29EA127}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1444,6 +1539,358 @@
         <v>1891250</v>
       </c>
     </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>44507</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>638336</v>
+      </c>
+      <c r="D29" s="2">
+        <v>7003983</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5966466</v>
+      </c>
+      <c r="F29" s="2">
+        <v>7472177</v>
+      </c>
+      <c r="G29" s="2">
+        <v>8205091</v>
+      </c>
+      <c r="H29" s="2">
+        <v>6815551</v>
+      </c>
+      <c r="I29" s="6">
+        <v>3522193</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1894026</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>44514</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
+        <v>943799</v>
+      </c>
+      <c r="D30" s="2">
+        <v>7049705</v>
+      </c>
+      <c r="E30" s="2">
+        <v>6001637</v>
+      </c>
+      <c r="F30" s="2">
+        <v>7496076</v>
+      </c>
+      <c r="G30" s="2">
+        <v>8221278</v>
+      </c>
+      <c r="H30" s="2">
+        <v>6825026</v>
+      </c>
+      <c r="I30" s="2">
+        <v>3525899</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1896858</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>44521</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1102068</v>
+      </c>
+      <c r="D31" s="2">
+        <v>7089549</v>
+      </c>
+      <c r="E31" s="2">
+        <v>6032737</v>
+      </c>
+      <c r="F31" s="2">
+        <v>7516013</v>
+      </c>
+      <c r="G31" s="2">
+        <v>8234211</v>
+      </c>
+      <c r="H31" s="2">
+        <v>6833304</v>
+      </c>
+      <c r="I31" s="2">
+        <v>3529309</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1899929</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1276908</v>
+      </c>
+      <c r="D32" s="2">
+        <v>7120064</v>
+      </c>
+      <c r="E32" s="2">
+        <v>6058190</v>
+      </c>
+      <c r="F32" s="2">
+        <v>7532339</v>
+      </c>
+      <c r="G32" s="2">
+        <v>8245285</v>
+      </c>
+      <c r="H32" s="2">
+        <v>6840748</v>
+      </c>
+      <c r="I32" s="2">
+        <v>3532774</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1903817</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>44535</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1337452</v>
+      </c>
+      <c r="D33" s="2">
+        <v>7152140</v>
+      </c>
+      <c r="E33" s="2">
+        <v>6086943</v>
+      </c>
+      <c r="F33" s="2">
+        <v>7550723</v>
+      </c>
+      <c r="G33" s="2">
+        <v>8257031</v>
+      </c>
+      <c r="H33" s="2">
+        <v>6848715</v>
+      </c>
+      <c r="I33" s="2">
+        <v>3536564</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1907422</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1447164</v>
+      </c>
+      <c r="D34" s="2">
+        <v>7207983</v>
+      </c>
+      <c r="E34" s="2">
+        <v>6134046</v>
+      </c>
+      <c r="F34" s="2">
+        <v>7579981</v>
+      </c>
+      <c r="G34" s="2">
+        <v>8273659</v>
+      </c>
+      <c r="H34" s="2">
+        <v>6859922</v>
+      </c>
+      <c r="I34" s="2">
+        <v>3541486</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1912406</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>44549</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="6">
+        <v>1687658</v>
+      </c>
+      <c r="D35" s="2">
+        <v>7292498</v>
+      </c>
+      <c r="E35" s="2">
+        <v>6210892</v>
+      </c>
+      <c r="F35" s="2">
+        <v>7634377</v>
+      </c>
+      <c r="G35" s="2">
+        <v>8309628</v>
+      </c>
+      <c r="H35" s="2">
+        <v>6882122</v>
+      </c>
+      <c r="I35" s="2">
+        <v>3549463</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1919442</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>44556</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1922603</v>
+      </c>
+      <c r="D36" s="2">
+        <v>7372485</v>
+      </c>
+      <c r="E36" s="2">
+        <v>6277067</v>
+      </c>
+      <c r="F36" s="2">
+        <v>7680835</v>
+      </c>
+      <c r="G36" s="2">
+        <v>8342124</v>
+      </c>
+      <c r="H36" s="2">
+        <v>6901646</v>
+      </c>
+      <c r="I36" s="2">
+        <v>3556497</v>
+      </c>
+      <c r="J36" s="2">
+        <v>1926010</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>44563</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2078387</v>
+      </c>
+      <c r="D37" s="2">
+        <v>7416478</v>
+      </c>
+      <c r="E37" s="7">
+        <v>6315105</v>
+      </c>
+      <c r="F37" s="7">
+        <v>7707497</v>
+      </c>
+      <c r="G37" s="7">
+        <v>8361449</v>
+      </c>
+      <c r="H37" s="7">
+        <v>6913206</v>
+      </c>
+      <c r="I37" s="7">
+        <v>3560716</v>
+      </c>
+      <c r="J37" s="7">
+        <v>1929885</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>44570</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2609927</v>
+      </c>
+      <c r="D38" s="3">
+        <v>6277566</v>
+      </c>
+      <c r="E38" s="3">
+        <v>6270149</v>
+      </c>
+      <c r="F38" s="3">
+        <v>7647467</v>
+      </c>
+      <c r="G38" s="8">
+        <v>8379513</v>
+      </c>
+      <c r="H38" s="8">
+        <v>7214833</v>
+      </c>
+      <c r="I38" s="8">
+        <v>3734894</v>
+      </c>
+      <c r="J38" s="8">
+        <v>2224143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>44577</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3">
+        <v>2652937</v>
+      </c>
+      <c r="D39" s="3">
+        <v>6295952</v>
+      </c>
+      <c r="E39" s="3">
+        <v>6294071</v>
+      </c>
+      <c r="F39" s="3">
+        <v>7664065</v>
+      </c>
+      <c r="G39" s="8">
+        <v>8392498</v>
+      </c>
+      <c r="H39" s="8">
+        <v>7222453</v>
+      </c>
+      <c r="I39" s="8">
+        <v>3737269</v>
+      </c>
+      <c r="J39" s="8">
+        <v>2225561</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1453,10 +1900,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA06488B-6AE1-6D45-B18E-AB20070D0C15}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2324,10 +2771,1079 @@
         <v>1840610</v>
       </c>
     </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>44507</v>
+      </c>
+      <c r="B29" s="9">
+        <f>'[1]2nd dose_prev'!B29-[1]Sheet4!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>16919</v>
+      </c>
+      <c r="D29" s="2">
+        <v>6532396</v>
+      </c>
+      <c r="E29" s="2">
+        <v>4657059</v>
+      </c>
+      <c r="F29" s="2">
+        <v>6844317</v>
+      </c>
+      <c r="G29" s="2">
+        <v>7866543</v>
+      </c>
+      <c r="H29" s="2">
+        <v>6618556</v>
+      </c>
+      <c r="I29" s="2">
+        <v>3462816</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1844627</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>44514</v>
+      </c>
+      <c r="B30" s="9">
+        <f>'[1]2nd dose_prev'!B30-[1]Sheet4!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
+        <v>203300</v>
+      </c>
+      <c r="D30" s="2">
+        <v>6703758</v>
+      </c>
+      <c r="E30" s="2">
+        <v>4794510</v>
+      </c>
+      <c r="F30" s="2">
+        <v>6966359</v>
+      </c>
+      <c r="G30" s="2">
+        <v>7958783</v>
+      </c>
+      <c r="H30" s="2">
+        <v>6660197</v>
+      </c>
+      <c r="I30" s="2">
+        <v>3475148</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1852313</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>44521</v>
+      </c>
+      <c r="B31" s="9">
+        <f>'[1]2nd dose_prev'!B31-[1]Sheet4!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
+        <v>372202</v>
+      </c>
+      <c r="D31" s="2">
+        <v>6779056</v>
+      </c>
+      <c r="E31" s="2">
+        <v>4850887</v>
+      </c>
+      <c r="F31" s="2">
+        <v>7009683</v>
+      </c>
+      <c r="G31" s="2">
+        <v>7985960</v>
+      </c>
+      <c r="H31" s="2">
+        <v>6674386</v>
+      </c>
+      <c r="I31" s="2">
+        <v>3480385</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1856031</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B32" s="9">
+        <f>'[1]2nd dose_prev'!B32-[1]Sheet4!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>588629</v>
+      </c>
+      <c r="D32" s="2">
+        <v>6845463</v>
+      </c>
+      <c r="E32" s="2">
+        <v>4898200</v>
+      </c>
+      <c r="F32" s="2">
+        <v>7044129</v>
+      </c>
+      <c r="G32" s="2">
+        <v>8007387</v>
+      </c>
+      <c r="H32" s="2">
+        <v>6687008</v>
+      </c>
+      <c r="I32" s="2">
+        <v>3485366</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1859979</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>44535</v>
+      </c>
+      <c r="B33" s="9">
+        <f>'[1]2nd dose_prev'!B33-[1]Sheet4!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="2">
+        <v>864086</v>
+      </c>
+      <c r="D33" s="2">
+        <v>6899927</v>
+      </c>
+      <c r="E33" s="2">
+        <v>4938982</v>
+      </c>
+      <c r="F33" s="2">
+        <v>7073535</v>
+      </c>
+      <c r="G33" s="2">
+        <v>8026256</v>
+      </c>
+      <c r="H33" s="2">
+        <v>6698539</v>
+      </c>
+      <c r="I33" s="2">
+        <v>3490001</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1863758</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B34" s="9">
+        <f>'[1]2nd dose_prev'!B34-[1]Sheet4!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1029602</v>
+      </c>
+      <c r="D34" s="2">
+        <v>6964968</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4984150</v>
+      </c>
+      <c r="F34" s="2">
+        <v>7104349</v>
+      </c>
+      <c r="G34" s="2">
+        <v>8044998</v>
+      </c>
+      <c r="H34" s="2">
+        <v>6710488</v>
+      </c>
+      <c r="I34" s="2">
+        <v>3494870</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1867548</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>44549</v>
+      </c>
+      <c r="B35" s="9">
+        <f>'[1]2nd dose_prev'!B35-[1]Sheet4!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1212371</v>
+      </c>
+      <c r="D35" s="2">
+        <v>7035429</v>
+      </c>
+      <c r="E35" s="2">
+        <v>5032934</v>
+      </c>
+      <c r="F35" s="2">
+        <v>7139533</v>
+      </c>
+      <c r="G35" s="2">
+        <v>8067471</v>
+      </c>
+      <c r="H35" s="2">
+        <v>6723655</v>
+      </c>
+      <c r="I35" s="2">
+        <v>3499907</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1871972</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>44556</v>
+      </c>
+      <c r="B36" s="9">
+        <f>'[1]2nd dose_prev'!B36-[1]Sheet4!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1296387</v>
+      </c>
+      <c r="D36" s="2">
+        <v>7089098</v>
+      </c>
+      <c r="E36" s="2">
+        <v>5072064</v>
+      </c>
+      <c r="F36" s="2">
+        <v>7167752</v>
+      </c>
+      <c r="G36" s="2">
+        <v>8086635</v>
+      </c>
+      <c r="H36" s="2">
+        <v>6734899</v>
+      </c>
+      <c r="I36" s="2">
+        <v>3504758</v>
+      </c>
+      <c r="J36" s="2">
+        <v>1876204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>44563</v>
+      </c>
+      <c r="B37" s="9">
+        <f>'[1]2nd dose_prev'!B37-[1]Sheet4!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1405077</v>
+      </c>
+      <c r="D37" s="2">
+        <v>7151266</v>
+      </c>
+      <c r="E37" s="2">
+        <v>5117795</v>
+      </c>
+      <c r="F37" s="2">
+        <v>7199300</v>
+      </c>
+      <c r="G37" s="2">
+        <v>8106295</v>
+      </c>
+      <c r="H37" s="2">
+        <v>6746511</v>
+      </c>
+      <c r="I37" s="2">
+        <v>3509677</v>
+      </c>
+      <c r="J37" s="2">
+        <v>1880931</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>44570</v>
+      </c>
+      <c r="B38" s="9">
+        <f>'[1]2nd dose_prev'!B38-[1]Sheet4!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2090622</v>
+      </c>
+      <c r="D38" s="3">
+        <v>6092609</v>
+      </c>
+      <c r="E38" s="3">
+        <v>5113082</v>
+      </c>
+      <c r="F38" s="3">
+        <v>7164881</v>
+      </c>
+      <c r="G38" s="2">
+        <v>8141289</v>
+      </c>
+      <c r="H38" s="2">
+        <v>7059382</v>
+      </c>
+      <c r="I38" s="2">
+        <v>3692024</v>
+      </c>
+      <c r="J38" s="2">
+        <v>2187334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>44577</v>
+      </c>
+      <c r="B39" s="9">
+        <f>'[1]2nd dose_prev'!B39-[1]Sheet4!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="3">
+        <v>2311093</v>
+      </c>
+      <c r="D39" s="3">
+        <v>6157579</v>
+      </c>
+      <c r="E39" s="3">
+        <v>5184196</v>
+      </c>
+      <c r="F39" s="3">
+        <v>7217069</v>
+      </c>
+      <c r="G39" s="2">
+        <v>8176400</v>
+      </c>
+      <c r="H39" s="2">
+        <v>7080625</v>
+      </c>
+      <c r="I39" s="2">
+        <v>3699116</v>
+      </c>
+      <c r="J39" s="2">
+        <v>2193185</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DBD868-DB03-1D4E-9CD9-0AF923D76D5A}">
+  <dimension ref="A1:J39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>44326</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>44333</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>44347</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>44382</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>44389</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>44403</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>44417</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>44431</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>44438</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>44445</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>44452</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>44459</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>44466</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>44473</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>44480</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>44487</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>44494</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>44500</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>44507</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>44514</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>44521</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>44535</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>111868</v>
+      </c>
+      <c r="E33" s="2">
+        <v>650516</v>
+      </c>
+      <c r="F33" s="2">
+        <v>378469</v>
+      </c>
+      <c r="G33" s="2">
+        <v>363187</v>
+      </c>
+      <c r="H33" s="2">
+        <v>499946</v>
+      </c>
+      <c r="I33" s="2">
+        <v>938654</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1009969</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>202261</v>
+      </c>
+      <c r="E34" s="2">
+        <v>774942</v>
+      </c>
+      <c r="F34" s="2">
+        <v>495753</v>
+      </c>
+      <c r="G34" s="2">
+        <v>516884</v>
+      </c>
+      <c r="H34" s="2">
+        <v>1397885</v>
+      </c>
+      <c r="I34" s="2">
+        <v>1657099</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1302398</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>44549</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>517326</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1104516</v>
+      </c>
+      <c r="F35" s="2">
+        <v>968477</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1494407</v>
+      </c>
+      <c r="H35" s="2">
+        <v>3370949</v>
+      </c>
+      <c r="I35" s="2">
+        <v>2576538</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1495926</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>44556</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <v>918202</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1347951</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1351568</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2397420</v>
+      </c>
+      <c r="H36" s="2">
+        <v>4649390</v>
+      </c>
+      <c r="I36" s="2">
+        <v>2947575</v>
+      </c>
+      <c r="J36" s="2">
+        <v>1583362</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>44563</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="7">
+        <v>1348579</v>
+      </c>
+      <c r="E37" s="7">
+        <v>1588783</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1770109</v>
+      </c>
+      <c r="G37" s="7">
+        <v>3603142</v>
+      </c>
+      <c r="H37" s="7">
+        <v>5407575</v>
+      </c>
+      <c r="I37" s="7">
+        <v>3128540</v>
+      </c>
+      <c r="J37" s="7">
+        <v>1630020</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>44570</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="8">
+        <v>242143</v>
+      </c>
+      <c r="D38" s="8">
+        <v>1389418</v>
+      </c>
+      <c r="E38" s="8">
+        <v>1734961</v>
+      </c>
+      <c r="F38" s="8">
+        <v>2208254</v>
+      </c>
+      <c r="G38" s="8">
+        <v>4296934</v>
+      </c>
+      <c r="H38" s="8">
+        <v>5820966</v>
+      </c>
+      <c r="I38" s="8">
+        <v>3355197</v>
+      </c>
+      <c r="J38" s="8">
+        <v>1968224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>44577</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39" s="8">
+        <v>272535</v>
+      </c>
+      <c r="D39" s="8">
+        <v>1757864</v>
+      </c>
+      <c r="E39" s="8">
+        <v>2048800</v>
+      </c>
+      <c r="F39" s="8">
+        <v>2764362</v>
+      </c>
+      <c r="G39" s="8">
+        <v>5042316</v>
+      </c>
+      <c r="H39" s="8">
+        <v>6051925</v>
+      </c>
+      <c r="I39" s="8">
+        <v>3409479</v>
+      </c>
+      <c r="J39" s="8">
+        <v>1989797</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add zeros to 3rd vaccination before 2021/12/05
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccination_12dose_05031031.xlsx
+++ b/data/vaccine/vaccination_12dose_05031031.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjlee/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7A784E-8E6C-7241-9C8E-DC66A3E35265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F514FD-8327-4F41-8E92-499DD9A54344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8600" yWindow="620" windowWidth="28800" windowHeight="15740" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" activeTab="2" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
   </bookViews>
   <sheets>
     <sheet name="1st dose" sheetId="1" r:id="rId1"/>
@@ -96,35 +96,6 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={64D7B1B1-E6AF-F24D-9648-FE478B623C74}</author>
-    <author>tc={C7F97C34-3911-E94C-817A-1FDE668F5392}</author>
-  </authors>
-  <commentList>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{64D7B1B1-E6AF-F24D-9648-FE478B623C74}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    12-17세: 12,596
-미포함</t>
-      </text>
-    </comment>
-    <comment ref="D19" authorId="1" shapeId="0" xr:uid="{C7F97C34-3911-E94C-817A-1FDE668F5392}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    12-17세: 13,051
-미포함</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
@@ -165,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -199,12 +170,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -617,25 +582,12 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D18" dT="2021-09-03T10:28:52.34" personId="{11A4F5F0-4273-964A-87D2-52A5A4679086}" id="{64D7B1B1-E6AF-F24D-9648-FE478B623C74}">
-    <text>12-17세: 12,596
-미포함</text>
-  </threadedComment>
-  <threadedComment ref="D19" dT="2021-09-03T10:31:16.26" personId="{11A4F5F0-4273-964A-87D2-52A5A4679086}" id="{C7F97C34-3911-E94C-817A-1FDE668F5392}">
-    <text>12-17세: 13,051
-미포함</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2E4180-383F-D540-B7B7-6029C29EA127}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1902,7 +1854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA06488B-6AE1-6D45-B18E-AB20070D0C15}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:J39"/>
     </sheetView>
   </sheetViews>
@@ -3143,11 +3095,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DBD868-DB03-1D4E-9CD9-0AF923D76D5A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DBD868-DB03-1D4E-9CD9-0AF923D76D5A}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3188,435 +3140,993 @@
       <c r="A2" s="1">
         <v>44319</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44326</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44333</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44340</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44347</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44354</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44361</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44368</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44375</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44382</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44389</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44396</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44403</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44410</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44417</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44424</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44431</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44438</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44445</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44452</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44459</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44466</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>44473</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>44480</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44487</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>44494</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>44500</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>44507</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>44514</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>44521</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>44528</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -3844,6 +4354,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
delete dates before 2021/11/25
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccination_12dose_05031031.xlsx
+++ b/data/vaccine/vaccination_12dose_05031031.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjlee/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F514FD-8327-4F41-8E92-499DD9A54344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C047D9F9-3D3F-F848-AE5A-33F05CBF7E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" activeTab="2" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
+    <workbookView xWindow="9280" yWindow="500" windowWidth="28800" windowHeight="15740" activeTab="2" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
   </bookViews>
   <sheets>
     <sheet name="1st dose" sheetId="1" r:id="rId1"/>
@@ -199,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -210,6 +210,7 @@
     <xf numFmtId="41" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -586,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2E4180-383F-D540-B7B7-6029C29EA127}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1428,7 +1429,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+      <c r="A27" s="10">
         <v>44494</v>
       </c>
       <c r="B27" s="5">
@@ -1460,7 +1461,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+      <c r="A28" s="10">
         <v>44500</v>
       </c>
       <c r="B28" s="5">
@@ -1855,7 +1856,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J39"/>
+      <selection activeCell="A27" sqref="A27:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2646,7 +2647,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+      <c r="A27" s="10">
         <v>44494</v>
       </c>
       <c r="B27" s="2">
@@ -2685,7 +2686,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+      <c r="A28" s="10">
         <v>44500</v>
       </c>
       <c r="B28" s="2">
@@ -3096,10 +3097,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DBD868-DB03-1D4E-9CD9-0AF923D76D5A}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3138,7 +3139,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44319</v>
+        <v>44525</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3146,31 +3147,31 @@
       <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
+      <c r="D2" s="7">
+        <v>53037</v>
+      </c>
+      <c r="E2" s="7">
+        <v>459349</v>
+      </c>
+      <c r="F2" s="7">
+        <v>241142</v>
+      </c>
+      <c r="G2" s="7">
+        <v>217165</v>
+      </c>
+      <c r="H2" s="7">
+        <v>246925</v>
+      </c>
+      <c r="I2" s="7">
+        <v>470185</v>
+      </c>
+      <c r="J2" s="7">
+        <v>575785</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44326</v>
+        <v>44535</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -3179,30 +3180,30 @@
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>0</v>
+        <v>111868</v>
       </c>
       <c r="E3" s="2">
-        <v>0</v>
+        <v>650516</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>378469</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>363187</v>
       </c>
       <c r="H3" s="2">
-        <v>0</v>
+        <v>499946</v>
       </c>
       <c r="I3" s="2">
-        <v>0</v>
+        <v>938654</v>
       </c>
       <c r="J3" s="2">
-        <v>0</v>
+        <v>1009969</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>44333</v>
+        <v>44542</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -3211,30 +3212,30 @@
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>202261</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
+        <v>774942</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>495753</v>
       </c>
       <c r="G4" s="2">
-        <v>0</v>
+        <v>516884</v>
       </c>
       <c r="H4" s="2">
-        <v>0</v>
+        <v>1397885</v>
       </c>
       <c r="I4" s="2">
-        <v>0</v>
+        <v>1657099</v>
       </c>
       <c r="J4" s="2">
-        <v>0</v>
+        <v>1302398</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>44340</v>
+        <v>44549</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -3243,30 +3244,30 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>517326</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>1104516</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>968477</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>1494407</v>
       </c>
       <c r="H5" s="2">
-        <v>0</v>
+        <v>3370949</v>
       </c>
       <c r="I5" s="2">
-        <v>0</v>
+        <v>2576538</v>
       </c>
       <c r="J5" s="2">
-        <v>0</v>
+        <v>1495926</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44347</v>
+        <v>44556</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -3275,30 +3276,30 @@
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>0</v>
+        <v>918202</v>
       </c>
       <c r="E6" s="2">
-        <v>0</v>
+        <v>1347951</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>1351568</v>
       </c>
       <c r="G6" s="2">
-        <v>0</v>
+        <v>2397420</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>4649390</v>
       </c>
       <c r="I6" s="2">
-        <v>0</v>
+        <v>2947575</v>
       </c>
       <c r="J6" s="2">
-        <v>0</v>
+        <v>1583362</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44354</v>
+        <v>44563</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -3306,1049 +3307,89 @@
       <c r="C7" s="2">
         <v>0</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0</v>
+      <c r="D7" s="7">
+        <v>1348579</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1588783</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1770109</v>
+      </c>
+      <c r="G7" s="7">
+        <v>3603142</v>
+      </c>
+      <c r="H7" s="7">
+        <v>5407575</v>
+      </c>
+      <c r="I7" s="7">
+        <v>3128540</v>
+      </c>
+      <c r="J7" s="7">
+        <v>1630020</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44361</v>
+        <v>44570</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
       </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0</v>
+      <c r="C8" s="8">
+        <v>242143</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1389418</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1734961</v>
+      </c>
+      <c r="F8" s="8">
+        <v>2208254</v>
+      </c>
+      <c r="G8" s="8">
+        <v>4296934</v>
+      </c>
+      <c r="H8" s="8">
+        <v>5820966</v>
+      </c>
+      <c r="I8" s="8">
+        <v>3355197</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1968224</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44368</v>
+        <v>44577</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
       </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>44375</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>44382</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>44389</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>44396</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>44403</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>44410</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>44417</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>44424</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>44431</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>44438</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>44445</v>
-      </c>
-      <c r="B20" s="2">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0</v>
-      </c>
-      <c r="G20" s="2">
-        <v>0</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>44452</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2">
-        <v>0</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0</v>
-      </c>
-      <c r="J21" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>44459</v>
-      </c>
-      <c r="B22" s="2">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>44466</v>
-      </c>
-      <c r="B23" s="2">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>44473</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0</v>
-      </c>
-      <c r="I24" s="2">
-        <v>0</v>
-      </c>
-      <c r="J24" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>44480</v>
-      </c>
-      <c r="B25" s="2">
-        <v>0</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0</v>
-      </c>
-      <c r="I25" s="2">
-        <v>0</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>44487</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0</v>
-      </c>
-      <c r="I26" s="2">
-        <v>0</v>
-      </c>
-      <c r="J26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>44494</v>
-      </c>
-      <c r="B27" s="2">
-        <v>0</v>
-      </c>
-      <c r="C27" s="2">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0</v>
-      </c>
-      <c r="I27" s="2">
-        <v>0</v>
-      </c>
-      <c r="J27" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>44500</v>
-      </c>
-      <c r="B28" s="2">
-        <v>0</v>
-      </c>
-      <c r="C28" s="2">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0</v>
-      </c>
-      <c r="G28" s="2">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0</v>
-      </c>
-      <c r="I28" s="2">
-        <v>0</v>
-      </c>
-      <c r="J28" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>44507</v>
-      </c>
-      <c r="B29" s="2">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2">
-        <v>0</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0</v>
-      </c>
-      <c r="G29" s="2">
-        <v>0</v>
-      </c>
-      <c r="H29" s="2">
-        <v>0</v>
-      </c>
-      <c r="I29" s="2">
-        <v>0</v>
-      </c>
-      <c r="J29" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>44514</v>
-      </c>
-      <c r="B30" s="2">
-        <v>0</v>
-      </c>
-      <c r="C30" s="2">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0</v>
-      </c>
-      <c r="I30" s="2">
-        <v>0</v>
-      </c>
-      <c r="J30" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>44521</v>
-      </c>
-      <c r="B31" s="2">
-        <v>0</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
-      <c r="I31" s="2">
-        <v>0</v>
-      </c>
-      <c r="J31" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>44528</v>
-      </c>
-      <c r="B32" s="2">
-        <v>0</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
-      <c r="I32" s="2">
-        <v>0</v>
-      </c>
-      <c r="J32" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>44535</v>
-      </c>
-      <c r="B33" s="2">
-        <v>0</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <v>111868</v>
-      </c>
-      <c r="E33" s="2">
-        <v>650516</v>
-      </c>
-      <c r="F33" s="2">
-        <v>378469</v>
-      </c>
-      <c r="G33" s="2">
-        <v>363187</v>
-      </c>
-      <c r="H33" s="2">
-        <v>499946</v>
-      </c>
-      <c r="I33" s="2">
-        <v>938654</v>
-      </c>
-      <c r="J33" s="2">
-        <v>1009969</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>44542</v>
-      </c>
-      <c r="B34" s="2">
-        <v>0</v>
-      </c>
-      <c r="C34" s="2">
-        <v>0</v>
-      </c>
-      <c r="D34" s="2">
-        <v>202261</v>
-      </c>
-      <c r="E34" s="2">
-        <v>774942</v>
-      </c>
-      <c r="F34" s="2">
-        <v>495753</v>
-      </c>
-      <c r="G34" s="2">
-        <v>516884</v>
-      </c>
-      <c r="H34" s="2">
-        <v>1397885</v>
-      </c>
-      <c r="I34" s="2">
-        <v>1657099</v>
-      </c>
-      <c r="J34" s="2">
-        <v>1302398</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>44549</v>
-      </c>
-      <c r="B35" s="2">
-        <v>0</v>
-      </c>
-      <c r="C35" s="2">
-        <v>0</v>
-      </c>
-      <c r="D35" s="2">
-        <v>517326</v>
-      </c>
-      <c r="E35" s="2">
-        <v>1104516</v>
-      </c>
-      <c r="F35" s="2">
-        <v>968477</v>
-      </c>
-      <c r="G35" s="2">
-        <v>1494407</v>
-      </c>
-      <c r="H35" s="2">
-        <v>3370949</v>
-      </c>
-      <c r="I35" s="2">
-        <v>2576538</v>
-      </c>
-      <c r="J35" s="2">
-        <v>1495926</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>44556</v>
-      </c>
-      <c r="B36" s="2">
-        <v>0</v>
-      </c>
-      <c r="C36" s="2">
-        <v>0</v>
-      </c>
-      <c r="D36" s="2">
-        <v>918202</v>
-      </c>
-      <c r="E36" s="2">
-        <v>1347951</v>
-      </c>
-      <c r="F36" s="2">
-        <v>1351568</v>
-      </c>
-      <c r="G36" s="2">
-        <v>2397420</v>
-      </c>
-      <c r="H36" s="2">
-        <v>4649390</v>
-      </c>
-      <c r="I36" s="2">
-        <v>2947575</v>
-      </c>
-      <c r="J36" s="2">
-        <v>1583362</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>44563</v>
-      </c>
-      <c r="B37" s="2">
-        <v>0</v>
-      </c>
-      <c r="C37" s="2">
-        <v>0</v>
-      </c>
-      <c r="D37" s="7">
-        <v>1348579</v>
-      </c>
-      <c r="E37" s="7">
-        <v>1588783</v>
-      </c>
-      <c r="F37" s="7">
-        <v>1770109</v>
-      </c>
-      <c r="G37" s="7">
-        <v>3603142</v>
-      </c>
-      <c r="H37" s="7">
-        <v>5407575</v>
-      </c>
-      <c r="I37" s="7">
-        <v>3128540</v>
-      </c>
-      <c r="J37" s="7">
-        <v>1630020</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>44570</v>
-      </c>
-      <c r="B38" s="2">
-        <v>0</v>
-      </c>
-      <c r="C38" s="8">
-        <v>242143</v>
-      </c>
-      <c r="D38" s="8">
-        <v>1389418</v>
-      </c>
-      <c r="E38" s="8">
-        <v>1734961</v>
-      </c>
-      <c r="F38" s="8">
-        <v>2208254</v>
-      </c>
-      <c r="G38" s="8">
-        <v>4296934</v>
-      </c>
-      <c r="H38" s="8">
-        <v>5820966</v>
-      </c>
-      <c r="I38" s="8">
-        <v>3355197</v>
-      </c>
-      <c r="J38" s="8">
-        <v>1968224</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>44577</v>
-      </c>
-      <c r="B39" s="2">
-        <v>0</v>
-      </c>
-      <c r="C39" s="8">
+      <c r="C9" s="8">
         <v>272535</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D9" s="8">
         <v>1757864</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E9" s="8">
         <v>2048800</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F9" s="8">
         <v>2764362</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G9" s="8">
         <v>5042316</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H9" s="8">
         <v>6051925</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I9" s="8">
         <v>3409479</v>
       </c>
-      <c r="J39" s="8">
+      <c r="J9" s="8">
         <v>1989797</v>
       </c>
     </row>

</xml_diff>